<commit_message>
Create medicine list flow document
</commit_message>
<xml_diff>
--- a/PharmacyManager/123456.xlsx
+++ b/PharmacyManager/123456.xlsx
@@ -59,7 +59,7 @@
     <t>Name3</t>
   </si>
   <si>
-    <t>Ketul</t>
+    <t>ml</t>
   </si>
 </sst>
 </file>
@@ -436,11 +436,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>